<commit_message>
Switched RawHeaderList from having a Type column to have a seperate column for each category a header might fulfil. This allows a single header line to fill multiple classification purposes.
Still unimplemented: handling of subheaders.
</commit_message>
<xml_diff>
--- a/FOIA SAR data/JSF/JSF Dec 2003 SAR Data Draw.xlsx
+++ b/FOIA SAR data/JSF/JSF Dec 2003 SAR Data Draw.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\2015-09 Joint Development\Research\JSF F-35\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Greg Sanders\Documents\Development\R-scripts-and-data\FOIA SAR data\JSF\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="12180" firstSheet="1" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="12180" firstSheet="1" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Cost Summary" sheetId="1" r:id="rId1"/>
@@ -594,7 +594,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1327,12 +1327,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
@@ -1341,6 +1335,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1474,6 +1474,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1509,6 +1526,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2653,13 +2687,13 @@
       <c r="C1" s="101"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="102" t="s">
+      <c r="A2" s="106" t="s">
         <v>55</v>
       </c>
-      <c r="B2" s="102"/>
-      <c r="C2" s="102"/>
-      <c r="D2" s="102"/>
-      <c r="E2" s="102"/>
+      <c r="B2" s="106"/>
+      <c r="C2" s="106"/>
+      <c r="D2" s="106"/>
+      <c r="E2" s="106"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="91" t="s">
@@ -3271,13 +3305,13 @@
       <c r="C29" s="101"/>
     </row>
     <row r="30" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="102" t="s">
+      <c r="A30" s="106" t="s">
         <v>55</v>
       </c>
-      <c r="B30" s="102"/>
-      <c r="C30" s="102"/>
-      <c r="D30" s="102"/>
-      <c r="E30" s="102"/>
+      <c r="B30" s="106"/>
+      <c r="C30" s="106"/>
+      <c r="D30" s="106"/>
+      <c r="E30" s="106"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="91" t="s">
@@ -3889,13 +3923,13 @@
       <c r="C57" s="101"/>
     </row>
     <row r="58" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="102" t="s">
+      <c r="A58" s="106" t="s">
         <v>64</v>
       </c>
-      <c r="B58" s="102"/>
-      <c r="C58" s="102"/>
-      <c r="D58" s="102"/>
-      <c r="E58" s="102"/>
+      <c r="B58" s="106"/>
+      <c r="C58" s="106"/>
+      <c r="D58" s="106"/>
+      <c r="E58" s="106"/>
     </row>
     <row r="59" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="91" t="s">
@@ -4481,13 +4515,13 @@
       <c r="C84" s="101"/>
     </row>
     <row r="85" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A85" s="102" t="s">
+      <c r="A85" s="106" t="s">
         <v>64</v>
       </c>
-      <c r="B85" s="102"/>
-      <c r="C85" s="102"/>
-      <c r="D85" s="102"/>
-      <c r="E85" s="102"/>
+      <c r="B85" s="106"/>
+      <c r="C85" s="106"/>
+      <c r="D85" s="106"/>
+      <c r="E85" s="106"/>
     </row>
     <row r="86" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="91" t="s">
@@ -5073,13 +5107,13 @@
       <c r="C111" s="101"/>
     </row>
     <row r="112" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A112" s="103" t="s">
+      <c r="A112" s="105" t="s">
         <v>66</v>
       </c>
-      <c r="B112" s="103"/>
-      <c r="C112" s="103"/>
-      <c r="D112" s="103"/>
-      <c r="E112" s="103"/>
+      <c r="B112" s="105"/>
+      <c r="C112" s="105"/>
+      <c r="D112" s="105"/>
+      <c r="E112" s="105"/>
     </row>
     <row r="113" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A113" s="91" t="s">
@@ -5613,13 +5647,13 @@
       <c r="C136" s="101"/>
     </row>
     <row r="137" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A137" s="103" t="s">
+      <c r="A137" s="105" t="s">
         <v>66</v>
       </c>
-      <c r="B137" s="103"/>
-      <c r="C137" s="103"/>
-      <c r="D137" s="103"/>
-      <c r="E137" s="103"/>
+      <c r="B137" s="105"/>
+      <c r="C137" s="105"/>
+      <c r="D137" s="105"/>
+      <c r="E137" s="105"/>
     </row>
     <row r="138" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A138" s="91" t="s">
@@ -7799,57 +7833,57 @@
       <c r="A257" s="91" t="s">
         <v>47</v>
       </c>
-      <c r="B257" s="104" t="s">
+      <c r="B257" s="102" t="s">
         <v>22</v>
       </c>
-      <c r="C257" s="104" t="s">
+      <c r="C257" s="102" t="s">
         <v>48</v>
       </c>
-      <c r="D257" s="104" t="s">
+      <c r="D257" s="102" t="s">
         <v>49</v>
       </c>
-      <c r="E257" s="104" t="s">
+      <c r="E257" s="102" t="s">
         <v>50</v>
       </c>
-      <c r="F257" s="104" t="s">
+      <c r="F257" s="102" t="s">
         <v>51</v>
       </c>
-      <c r="G257" s="104" t="s">
+      <c r="G257" s="102" t="s">
         <v>52</v>
       </c>
-      <c r="H257" s="104" t="s">
+      <c r="H257" s="102" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="258" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A258" s="92"/>
-      <c r="B258" s="105"/>
-      <c r="C258" s="105"/>
-      <c r="D258" s="105"/>
-      <c r="E258" s="105"/>
-      <c r="F258" s="105"/>
-      <c r="G258" s="105"/>
-      <c r="H258" s="105"/>
+      <c r="B258" s="103"/>
+      <c r="C258" s="103"/>
+      <c r="D258" s="103"/>
+      <c r="E258" s="103"/>
+      <c r="F258" s="103"/>
+      <c r="G258" s="103"/>
+      <c r="H258" s="103"/>
     </row>
     <row r="259" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A259" s="92"/>
-      <c r="B259" s="105"/>
-      <c r="C259" s="105"/>
-      <c r="D259" s="105"/>
-      <c r="E259" s="105"/>
-      <c r="F259" s="105"/>
-      <c r="G259" s="105"/>
-      <c r="H259" s="105"/>
+      <c r="B259" s="103"/>
+      <c r="C259" s="103"/>
+      <c r="D259" s="103"/>
+      <c r="E259" s="103"/>
+      <c r="F259" s="103"/>
+      <c r="G259" s="103"/>
+      <c r="H259" s="103"/>
     </row>
     <row r="260" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A260" s="93"/>
-      <c r="B260" s="106"/>
-      <c r="C260" s="106"/>
-      <c r="D260" s="106"/>
-      <c r="E260" s="106"/>
-      <c r="F260" s="106"/>
-      <c r="G260" s="106"/>
-      <c r="H260" s="106"/>
+      <c r="B260" s="104"/>
+      <c r="C260" s="104"/>
+      <c r="D260" s="104"/>
+      <c r="E260" s="104"/>
+      <c r="F260" s="104"/>
+      <c r="G260" s="104"/>
+      <c r="H260" s="104"/>
     </row>
     <row r="261" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A261" s="25">
@@ -8463,7 +8497,7 @@
       <c r="A287" s="91" t="s">
         <v>47</v>
       </c>
-      <c r="B287" s="104" t="s">
+      <c r="B287" s="102" t="s">
         <v>22</v>
       </c>
       <c r="C287" s="91" t="s">
@@ -8487,7 +8521,7 @@
     </row>
     <row r="288" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A288" s="92"/>
-      <c r="B288" s="105"/>
+      <c r="B288" s="103"/>
       <c r="C288" s="92"/>
       <c r="D288" s="92"/>
       <c r="E288" s="92"/>
@@ -8497,7 +8531,7 @@
     </row>
     <row r="289" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A289" s="92"/>
-      <c r="B289" s="105"/>
+      <c r="B289" s="103"/>
       <c r="C289" s="92"/>
       <c r="D289" s="92"/>
       <c r="E289" s="92"/>
@@ -8507,7 +8541,7 @@
     </row>
     <row r="290" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A290" s="93"/>
-      <c r="B290" s="106"/>
+      <c r="B290" s="104"/>
       <c r="C290" s="93"/>
       <c r="D290" s="93"/>
       <c r="E290" s="93"/>
@@ -9605,6 +9639,90 @@
     </row>
   </sheetData>
   <mergeCells count="108">
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A3:A6"/>
+    <mergeCell ref="B3:B6"/>
+    <mergeCell ref="C3:C6"/>
+    <mergeCell ref="D3:D6"/>
+    <mergeCell ref="E3:E6"/>
+    <mergeCell ref="F3:F6"/>
+    <mergeCell ref="A29:C29"/>
+    <mergeCell ref="A30:E30"/>
+    <mergeCell ref="A31:A34"/>
+    <mergeCell ref="B31:B34"/>
+    <mergeCell ref="C31:C34"/>
+    <mergeCell ref="D31:D34"/>
+    <mergeCell ref="E31:E34"/>
+    <mergeCell ref="G3:G6"/>
+    <mergeCell ref="H3:H6"/>
+    <mergeCell ref="F31:F34"/>
+    <mergeCell ref="G31:G34"/>
+    <mergeCell ref="H31:H34"/>
+    <mergeCell ref="A57:C57"/>
+    <mergeCell ref="A58:E58"/>
+    <mergeCell ref="A59:A62"/>
+    <mergeCell ref="B59:B62"/>
+    <mergeCell ref="C59:C62"/>
+    <mergeCell ref="D59:D62"/>
+    <mergeCell ref="E59:E62"/>
+    <mergeCell ref="F59:F62"/>
+    <mergeCell ref="G59:G62"/>
+    <mergeCell ref="H59:H62"/>
+    <mergeCell ref="A84:C84"/>
+    <mergeCell ref="A85:E85"/>
+    <mergeCell ref="A86:A89"/>
+    <mergeCell ref="B86:B89"/>
+    <mergeCell ref="C86:C89"/>
+    <mergeCell ref="D86:D89"/>
+    <mergeCell ref="E86:E89"/>
+    <mergeCell ref="F86:F89"/>
+    <mergeCell ref="G86:G89"/>
+    <mergeCell ref="H86:H89"/>
+    <mergeCell ref="A111:C111"/>
+    <mergeCell ref="A112:E112"/>
+    <mergeCell ref="A113:A116"/>
+    <mergeCell ref="B113:B116"/>
+    <mergeCell ref="C113:C116"/>
+    <mergeCell ref="D113:D116"/>
+    <mergeCell ref="E113:E116"/>
+    <mergeCell ref="F113:F116"/>
+    <mergeCell ref="G113:G116"/>
+    <mergeCell ref="H113:H116"/>
+    <mergeCell ref="A136:C136"/>
+    <mergeCell ref="A137:E137"/>
+    <mergeCell ref="A138:A141"/>
+    <mergeCell ref="B138:B141"/>
+    <mergeCell ref="C138:C141"/>
+    <mergeCell ref="D138:D141"/>
+    <mergeCell ref="E138:E141"/>
+    <mergeCell ref="F138:F141"/>
+    <mergeCell ref="G138:G141"/>
+    <mergeCell ref="H138:H141"/>
+    <mergeCell ref="G185:G188"/>
+    <mergeCell ref="H185:H188"/>
+    <mergeCell ref="G163:G166"/>
+    <mergeCell ref="H163:H166"/>
+    <mergeCell ref="A174:A177"/>
+    <mergeCell ref="B174:B177"/>
+    <mergeCell ref="C174:C177"/>
+    <mergeCell ref="D174:D177"/>
+    <mergeCell ref="E174:E177"/>
+    <mergeCell ref="F174:F177"/>
+    <mergeCell ref="G174:G177"/>
+    <mergeCell ref="H174:H177"/>
+    <mergeCell ref="A163:A166"/>
+    <mergeCell ref="B163:B166"/>
+    <mergeCell ref="C163:C166"/>
+    <mergeCell ref="D163:D166"/>
+    <mergeCell ref="E163:E166"/>
+    <mergeCell ref="F163:F166"/>
+    <mergeCell ref="A185:A188"/>
+    <mergeCell ref="B185:B188"/>
+    <mergeCell ref="C185:C188"/>
+    <mergeCell ref="D185:D188"/>
+    <mergeCell ref="E185:E188"/>
+    <mergeCell ref="F185:F188"/>
     <mergeCell ref="G287:G290"/>
     <mergeCell ref="H287:H290"/>
     <mergeCell ref="A287:A290"/>
@@ -9629,90 +9747,6 @@
     <mergeCell ref="D210:D213"/>
     <mergeCell ref="E210:E213"/>
     <mergeCell ref="F210:F213"/>
-    <mergeCell ref="G185:G188"/>
-    <mergeCell ref="H185:H188"/>
-    <mergeCell ref="G163:G166"/>
-    <mergeCell ref="H163:H166"/>
-    <mergeCell ref="A174:A177"/>
-    <mergeCell ref="B174:B177"/>
-    <mergeCell ref="C174:C177"/>
-    <mergeCell ref="D174:D177"/>
-    <mergeCell ref="E174:E177"/>
-    <mergeCell ref="F174:F177"/>
-    <mergeCell ref="G174:G177"/>
-    <mergeCell ref="H174:H177"/>
-    <mergeCell ref="A163:A166"/>
-    <mergeCell ref="B163:B166"/>
-    <mergeCell ref="C163:C166"/>
-    <mergeCell ref="D163:D166"/>
-    <mergeCell ref="E163:E166"/>
-    <mergeCell ref="F163:F166"/>
-    <mergeCell ref="A185:A188"/>
-    <mergeCell ref="B185:B188"/>
-    <mergeCell ref="C185:C188"/>
-    <mergeCell ref="D185:D188"/>
-    <mergeCell ref="E185:E188"/>
-    <mergeCell ref="F185:F188"/>
-    <mergeCell ref="H113:H116"/>
-    <mergeCell ref="A136:C136"/>
-    <mergeCell ref="A137:E137"/>
-    <mergeCell ref="A138:A141"/>
-    <mergeCell ref="B138:B141"/>
-    <mergeCell ref="C138:C141"/>
-    <mergeCell ref="D138:D141"/>
-    <mergeCell ref="E138:E141"/>
-    <mergeCell ref="F138:F141"/>
-    <mergeCell ref="G138:G141"/>
-    <mergeCell ref="H138:H141"/>
-    <mergeCell ref="A111:C111"/>
-    <mergeCell ref="A112:E112"/>
-    <mergeCell ref="A113:A116"/>
-    <mergeCell ref="B113:B116"/>
-    <mergeCell ref="C113:C116"/>
-    <mergeCell ref="D113:D116"/>
-    <mergeCell ref="E113:E116"/>
-    <mergeCell ref="F113:F116"/>
-    <mergeCell ref="G113:G116"/>
-    <mergeCell ref="H59:H62"/>
-    <mergeCell ref="A84:C84"/>
-    <mergeCell ref="A85:E85"/>
-    <mergeCell ref="A86:A89"/>
-    <mergeCell ref="B86:B89"/>
-    <mergeCell ref="C86:C89"/>
-    <mergeCell ref="D86:D89"/>
-    <mergeCell ref="E86:E89"/>
-    <mergeCell ref="F86:F89"/>
-    <mergeCell ref="G86:G89"/>
-    <mergeCell ref="H86:H89"/>
-    <mergeCell ref="A57:C57"/>
-    <mergeCell ref="A58:E58"/>
-    <mergeCell ref="A59:A62"/>
-    <mergeCell ref="B59:B62"/>
-    <mergeCell ref="C59:C62"/>
-    <mergeCell ref="D59:D62"/>
-    <mergeCell ref="E59:E62"/>
-    <mergeCell ref="F59:F62"/>
-    <mergeCell ref="G59:G62"/>
-    <mergeCell ref="A30:E30"/>
-    <mergeCell ref="A31:A34"/>
-    <mergeCell ref="B31:B34"/>
-    <mergeCell ref="C31:C34"/>
-    <mergeCell ref="D31:D34"/>
-    <mergeCell ref="E31:E34"/>
-    <mergeCell ref="G3:G6"/>
-    <mergeCell ref="H3:H6"/>
-    <mergeCell ref="F31:F34"/>
-    <mergeCell ref="G31:G34"/>
-    <mergeCell ref="H31:H34"/>
-    <mergeCell ref="A2:E2"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A3:A6"/>
-    <mergeCell ref="B3:B6"/>
-    <mergeCell ref="C3:C6"/>
-    <mergeCell ref="D3:D6"/>
-    <mergeCell ref="E3:E6"/>
-    <mergeCell ref="F3:F6"/>
-    <mergeCell ref="A29:C29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -10238,7 +10272,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
@@ -10609,8 +10643,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E81"/>
   <sheetViews>
-    <sheetView topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="C84" sqref="C84"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11511,7 +11545,7 @@
     <row r="61" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="62" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="73" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B62" s="116" t="s">
         <v>143</v>

</xml_diff>